<commit_message>
Revert "Update Excel table version of SDs of residuals + assoc. F-tests"
This reverts commit 6366ce86116e2da6338d71bec6dbfd4b41515c29.
</commit_message>
<xml_diff>
--- a/draft-02/manuscript_ver3-4/results/sd-of-residuals-w-and-wo-outliers.xlsx
+++ b/draft-02/manuscript_ver3-4/results/sd-of-residuals-w-and-wo-outliers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/draft-02/manuscript_ver3-4/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/draft-02/manuscript_ver3-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E6DA5A-79F2-C84F-8A5C-7A81E417B7CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AABB9-7479-F040-997B-7A3C046858CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="28100" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sd-of-residuals-w-and-wo-outlie" sheetId="1" r:id="rId1"/>
@@ -74,6 +74,48 @@
   </si>
   <si>
     <t>MV</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.466</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.337</t>
+    </r>
   </si>
   <si>
     <r>
@@ -97,48 +139,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> &lt; 0.01</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.064</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> =  0.059</t>
     </r>
   </si>
 </sst>
@@ -648,26 +648,34 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1026,7 +1034,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1040,7 +1048,6 @@
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="1.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="2" customWidth="1"/>
     <col min="11" max="11" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1051,43 +1058,43 @@
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="7" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1098,45 +1105,56 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.242554058371929</v>
-      </c>
-      <c r="E5">
-        <v>0.14085647439245699</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.21816783309028301</v>
-      </c>
-      <c r="I5">
-        <v>8.3887975815100393E-2</v>
+      <c r="C5" s="3">
+        <v>965.28729503194904</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>638.37698587611305</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="8">
+        <v>665.01669227496905</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="8">
+        <v>383.79310102008498</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.22308686776707101</v>
-      </c>
-      <c r="E6">
-        <v>0.109893196763538</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.22305467134160201</v>
-      </c>
-      <c r="I6">
-        <v>0.101396663837033</v>
+      <c r="C6" s="3">
+        <v>558.40948500263096</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>353.93076929915799</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="8">
+        <v>554.67920763353004</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="8">
+        <v>336.42885340761302</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1146,35 +1164,50 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>0.367090335353778</v>
-      </c>
-      <c r="E8">
-        <v>0.337298310861191</v>
-      </c>
-      <c r="G8">
-        <v>0.36456751376097002</v>
-      </c>
-      <c r="I8">
-        <v>0.337298310861191</v>
+      <c r="C8" s="3">
+        <v>607.10177186706801</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>540.16949843310999</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>467.825802826244</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
+        <v>437.30975150846899</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>0.329753504864358</v>
-      </c>
-      <c r="E9">
-        <v>0.29600485734805498</v>
-      </c>
-      <c r="G9">
-        <v>0.32407946910603402</v>
-      </c>
-      <c r="I9">
-        <v>0.29600485734805498</v>
-      </c>
+      <c r="C9" s="3">
+        <v>387.00494175833501</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>337.31179360655801</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>343.84351462341402</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
+        <v>299.518852067323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
@@ -1183,38 +1216,44 @@
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0.43169506174466898</v>
-      </c>
-      <c r="E11">
-        <v>0.40884340775186001</v>
-      </c>
-      <c r="G11">
-        <v>0.42598091255232401</v>
-      </c>
-      <c r="I11">
-        <v>0.404705623285396</v>
+      <c r="C11" s="3">
+        <v>335.17229652894201</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <v>315.519035929479</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
+        <v>233.44825894088399</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <v>222.597231636732</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C12">
-        <v>0.47335898491254902</v>
-      </c>
-      <c r="E12">
-        <v>0.44063714280504901</v>
-      </c>
-      <c r="G12">
-        <v>0.46811374560168401</v>
-      </c>
-      <c r="I12">
-        <v>0.42531564176075598</v>
+      <c r="C12" s="3">
+        <v>247.394864914263</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>230.05084730116499</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <v>198.35573980529</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
+        <v>174.12887031053799</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="I14" s="6"/>
+      <c r="I14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Update Excel table version of SDs of residuals + assoc. F-tests
</commit_message>
<xml_diff>
--- a/draft-02/manuscript_ver3-4/results/sd-of-residuals-w-and-wo-outliers.xlsx
+++ b/draft-02/manuscript_ver3-4/results/sd-of-residuals-w-and-wo-outliers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/draft-02/manuscript_ver3-4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/draft-02/manuscript_ver3-4/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AABB9-7479-F040-997B-7A3C046858CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E6DA5A-79F2-C84F-8A5C-7A81E417B7CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="28100" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sd-of-residuals-w-and-wo-outlie" sheetId="1" r:id="rId1"/>
@@ -74,48 +74,6 @@
   </si>
   <si>
     <t>MV</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.466</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.337</t>
-    </r>
   </si>
   <si>
     <r>
@@ -139,6 +97,48 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> &lt; 0.01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.064</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> =  0.059</t>
     </r>
   </si>
 </sst>
@@ -648,34 +648,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1034,7 +1026,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1048,6 +1040,7 @@
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="1.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="2" customWidth="1"/>
     <col min="11" max="11" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1058,43 +1051,43 @@
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="6" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1105,56 +1098,45 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
-        <v>965.28729503194904</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>638.37698587611305</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="8">
-        <v>665.01669227496905</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="8">
-        <v>383.79310102008498</v>
+      <c r="C5" s="5">
+        <v>0.242554058371929</v>
+      </c>
+      <c r="E5">
+        <v>0.14085647439245699</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.21816783309028301</v>
+      </c>
+      <c r="I5">
+        <v>8.3887975815100393E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
-        <v>558.40948500263096</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
-        <v>353.93076929915799</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="8">
-        <v>554.67920763353004</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="8">
-        <v>336.42885340761302</v>
+      <c r="C6" s="5">
+        <v>0.22308686776707101</v>
+      </c>
+      <c r="E6">
+        <v>0.109893196763538</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.22305467134160201</v>
+      </c>
+      <c r="I6">
+        <v>0.101396663837033</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="10" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10" t="s">
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1164,50 +1146,35 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3">
-        <v>607.10177186706801</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <v>540.16949843310999</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3">
-        <v>467.825802826244</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3">
-        <v>437.30975150846899</v>
+      <c r="C8">
+        <v>0.367090335353778</v>
+      </c>
+      <c r="E8">
+        <v>0.337298310861191</v>
+      </c>
+      <c r="G8">
+        <v>0.36456751376097002</v>
+      </c>
+      <c r="I8">
+        <v>0.337298310861191</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="3">
-        <v>387.00494175833501</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3">
-        <v>337.31179360655801</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3">
-        <v>343.84351462341402</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3">
-        <v>299.518852067323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="C9">
+        <v>0.329753504864358</v>
+      </c>
+      <c r="E9">
+        <v>0.29600485734805498</v>
+      </c>
+      <c r="G9">
+        <v>0.32407946910603402</v>
+      </c>
+      <c r="I9">
+        <v>0.29600485734805498</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
@@ -1216,44 +1183,38 @@
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3">
-        <v>335.17229652894201</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3">
-        <v>315.519035929479</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3">
-        <v>233.44825894088399</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3">
-        <v>222.597231636732</v>
+      <c r="C11">
+        <v>0.43169506174466898</v>
+      </c>
+      <c r="E11">
+        <v>0.40884340775186001</v>
+      </c>
+      <c r="G11">
+        <v>0.42598091255232401</v>
+      </c>
+      <c r="I11">
+        <v>0.404705623285396</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
-        <v>247.394864914263</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
-        <v>230.05084730116499</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3">
-        <v>198.35573980529</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3">
-        <v>174.12887031053799</v>
+      <c r="C12">
+        <v>0.47335898491254902</v>
+      </c>
+      <c r="E12">
+        <v>0.44063714280504901</v>
+      </c>
+      <c r="G12">
+        <v>0.46811374560168401</v>
+      </c>
+      <c r="I12">
+        <v>0.42531564176075598</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="I14" s="12"/>
+      <c r="I14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>